<commit_message>
updated model according to robinson advice and changed letters
</commit_message>
<xml_diff>
--- a/LMER_Analysis_Table.xlsx
+++ b/LMER_Analysis_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telec\OneDrive\Desktop\Current Projects\Steak_Cutting_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon Kim\OneDrive\Desktop\School Stuff\Steak_Cutting_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EF60ED-845B-43A6-ADF2-4A3FFEECCA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF4767C-661B-4B6B-82FE-649C5F236338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
   <si>
     <t>Muscle Type: LL</t>
   </si>
@@ -105,9 +105,6 @@
     <t>46.3e</t>
   </si>
   <si>
-    <t>47e</t>
-  </si>
-  <si>
     <t>Muscle Type: PM</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>52.8abc</t>
   </si>
   <si>
-    <t>52.4bc</t>
-  </si>
-  <si>
     <t>52.2bcd</t>
   </si>
   <si>
@@ -162,42 +156,12 @@
     <t>15.37c</t>
   </si>
   <si>
-    <t>14.71c</t>
-  </si>
-  <si>
     <t>10.08d</t>
   </si>
   <si>
     <t>9.98d</t>
   </si>
   <si>
-    <t>16.87a</t>
-  </si>
-  <si>
-    <t>17.02a</t>
-  </si>
-  <si>
-    <t>17.65ab</t>
-  </si>
-  <si>
-    <t>18.98b</t>
-  </si>
-  <si>
-    <t>14.61c</t>
-  </si>
-  <si>
-    <t>14.95c</t>
-  </si>
-  <si>
-    <t>11.69d</t>
-  </si>
-  <si>
-    <t>10.6d</t>
-  </si>
-  <si>
-    <t>8.44e</t>
-  </si>
-  <si>
     <t>7.18e</t>
   </si>
   <si>
@@ -207,54 +171,9 @@
     <t>7.58c</t>
   </si>
   <si>
-    <t>11.27b</t>
-  </si>
-  <si>
-    <t>9.46a</t>
-  </si>
-  <si>
-    <t>9.91a</t>
-  </si>
-  <si>
-    <t>9.51a</t>
-  </si>
-  <si>
-    <t>9.81a</t>
-  </si>
-  <si>
-    <t>9.77a</t>
-  </si>
-  <si>
-    <t>9.66a</t>
-  </si>
-  <si>
-    <t>6.71f</t>
-  </si>
-  <si>
-    <t>7.42ef</t>
-  </si>
-  <si>
-    <t>9.98a</t>
-  </si>
-  <si>
-    <t>10.87ab</t>
-  </si>
-  <si>
     <t>9.21bc</t>
   </si>
   <si>
-    <t>8.67cd</t>
-  </si>
-  <si>
-    <t>8.29cde</t>
-  </si>
-  <si>
-    <t>8.61cde</t>
-  </si>
-  <si>
-    <t>7.78def</t>
-  </si>
-  <si>
     <t>0.19a</t>
   </si>
   <si>
@@ -318,24 +237,9 @@
     <t>5.61a</t>
   </si>
   <si>
-    <t>5.57b</t>
-  </si>
-  <si>
-    <t>5.46c</t>
-  </si>
-  <si>
     <t>5.51bc</t>
   </si>
   <si>
-    <t>5.42c</t>
-  </si>
-  <si>
-    <t>5.47c</t>
-  </si>
-  <si>
-    <t>5.44c</t>
-  </si>
-  <si>
     <t>5.62a</t>
   </si>
   <si>
@@ -390,15 +294,9 @@
     <t>97.28d</t>
   </si>
   <si>
-    <t>5.22a</t>
-  </si>
-  <si>
     <t>4.91a</t>
   </si>
   <si>
-    <t>5.28a</t>
-  </si>
-  <si>
     <t>4.73a</t>
   </si>
   <si>
@@ -408,52 +306,160 @@
     <t>5.33ab</t>
   </si>
   <si>
-    <t>6.03bcd</t>
-  </si>
-  <si>
-    <t>6.18cd</t>
-  </si>
-  <si>
-    <t>5.39d</t>
-  </si>
-  <si>
-    <t>6.30d</t>
-  </si>
-  <si>
     <t>0.250a</t>
   </si>
   <si>
-    <t>8.50cde</t>
-  </si>
-  <si>
-    <t>9.60a</t>
-  </si>
-  <si>
     <t>2.51a</t>
   </si>
   <si>
-    <t>3.49bc</t>
-  </si>
-  <si>
     <t>2.98ab</t>
   </si>
   <si>
-    <t>3.60bcd</t>
-  </si>
-  <si>
-    <t>3.81cd</t>
-  </si>
-  <si>
-    <t>4.28d</t>
-  </si>
-  <si>
-    <t>5.04e</t>
-  </si>
-  <si>
-    <t>5.24e</t>
-  </si>
-  <si>
     <t>5.94f</t>
+  </si>
+  <si>
+    <t>47de</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>52.4abcd</t>
+  </si>
+  <si>
+    <t>14.71cd</t>
+  </si>
+  <si>
+    <t>8.44de</t>
+  </si>
+  <si>
+    <t>10.6cd</t>
+  </si>
+  <si>
+    <t>16.87ab</t>
+  </si>
+  <si>
+    <t>17.02ab</t>
+  </si>
+  <si>
+    <t>17.65a</t>
+  </si>
+  <si>
+    <t>18.98a</t>
+  </si>
+  <si>
+    <t>14.61b</t>
+  </si>
+  <si>
+    <t>14.95b</t>
+  </si>
+  <si>
+    <t>11.69c</t>
+  </si>
+  <si>
+    <t>11.27a</t>
+  </si>
+  <si>
+    <t>9.46b</t>
+  </si>
+  <si>
+    <t>9.51b</t>
+  </si>
+  <si>
+    <t>9.77b</t>
+  </si>
+  <si>
+    <t>9.81b</t>
+  </si>
+  <si>
+    <t>9.60b</t>
+  </si>
+  <si>
+    <t>9.66b</t>
+  </si>
+  <si>
+    <t>9.91ab</t>
+  </si>
+  <si>
+    <t>10.87a</t>
+  </si>
+  <si>
+    <t>9.98ab</t>
+  </si>
+  <si>
+    <t>8.67bcd</t>
+  </si>
+  <si>
+    <t>8.61bcd</t>
+  </si>
+  <si>
+    <t>8.50cd</t>
+  </si>
+  <si>
+    <t>8.29cd</t>
+  </si>
+  <si>
+    <t>7.78cde</t>
+  </si>
+  <si>
+    <t>7.42de</t>
+  </si>
+  <si>
+    <t>6.71e</t>
+  </si>
+  <si>
+    <t>5.57abc</t>
+  </si>
+  <si>
+    <t>5.51bcd</t>
+  </si>
+  <si>
+    <t>5.47cd</t>
+  </si>
+  <si>
+    <t>5.44d</t>
+  </si>
+  <si>
+    <t>5.42d</t>
+  </si>
+  <si>
+    <t>5.46d</t>
+  </si>
+  <si>
+    <t>5.22ab</t>
+  </si>
+  <si>
+    <t>5.28ab</t>
+  </si>
+  <si>
+    <t>6.03bc</t>
+  </si>
+  <si>
+    <t>6.18bc</t>
+  </si>
+  <si>
+    <t>6.30c</t>
+  </si>
+  <si>
+    <t>5.39c</t>
+  </si>
+  <si>
+    <t>3.49abc</t>
+  </si>
+  <si>
+    <t>3.60bc</t>
+  </si>
+  <si>
+    <t>3.81bc</t>
+  </si>
+  <si>
+    <t>4.28cd</t>
+  </si>
+  <si>
+    <t>5.04de</t>
+  </si>
+  <si>
+    <t>5.24ef</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,8 +488,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -584,11 +602,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,6 +644,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,21 +943,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,233 +982,256 @@
       <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="16">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="12"/>
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G5" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D6" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="16">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="16">
+        <v>7.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D10" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="16">
+        <v>5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>1</v>
@@ -1179,230 +1254,253 @@
       <c r="H13" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="16">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="16">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D17" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="16">
+        <v>7.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D22" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="16">
+        <v>5.0200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D23" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>1</v>
@@ -1425,96 +1523,107 @@
       <c r="H25" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+      <c r="I26" s="16">
+        <v>0.1915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0.58599999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>14</v>
       </c>
@@ -1522,44 +1631,81 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>140</v>
       </c>
+      <c r="F30" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>143</v>
+      </c>
       <c r="H30" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="I30" s="16">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>135</v>
+      <c r="D31" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="14" t="s">
         <v>141</v>
       </c>
+      <c r="G31" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="19"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="19"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="28">
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
@@ -1567,12 +1713,6 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>